<commit_message>
Added more s-dashboard e2e test
</commit_message>
<xml_diff>
--- a/web/WBTBSsystem/system/downloads/testOut.xlsx
+++ b/web/WBTBSsystem/system/downloads/testOut.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,32 +486,100 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>31</v>
+        <v>110</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CN0006</t>
+          <t>CN0004</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>OUTBOUND</t>
+          <t>INBOUND</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Scheduled</t>
+          <t>Confirmed</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" s="2" t="n">
+        <v>45376.14305555556</v>
+      </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve">NB002
+          <t xml:space="preserve">NB001
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>118</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CN0010</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>INBOUND</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" s="2" t="n">
+        <v>45376.14305555556</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NB001
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>111</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CN0005</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>INBOUND</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Scheduled</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NB001
 </t>
         </is>
       </c>

</xml_diff>